<commit_message>
Mark some fields, that can be missed in file as Optional. Correct some columns. Add parent model with sql related methods. Correct tests.
</commit_message>
<xml_diff>
--- a/src/parsebp/tests/regular.xlsx
+++ b/src/parsebp/tests/regular.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="18.04.2022_Pricelist_UA" sheetId="1" state="visible" r:id="rId2"/>
@@ -300,6 +300,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -435,8 +436,12 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -567,7 +572,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.02"/>
@@ -789,7 +794,7 @@
       </c>
       <c r="N5" s="7" t="n">
         <f aca="false">M5/L5-1</f>
-        <v>-0.0799773915500918</v>
+        <v>-0.0799773915500919</v>
       </c>
       <c r="O5" s="0" t="s">
         <v>23</v>
@@ -1044,7 +1049,7 @@
       </c>
       <c r="N11" s="7" t="n">
         <f aca="false">M11/L11-1</f>
-        <v>-0.0176104383421457</v>
+        <v>-0.0176104383421455</v>
       </c>
       <c r="O11" s="0" t="s">
         <v>23</v>
@@ -1075,7 +1080,7 @@
       <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1317,11 +1322,11 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
@@ -1730,7 +1735,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
@@ -1780,11 +1785,11 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">

</xml_diff>